<commit_message>
Se sube CU 13 - 15 - 16 - 17 full full
</commit_message>
<xml_diff>
--- a/se/Trabajo Profesional/Disciplinas/3.Analisis/Casos de Uso/CU15 - Modificando rutina de entrenamiento/TC15 - Modificando rutina de entrenamiento.xlsx
+++ b/se/Trabajo Profesional/Disciplinas/3.Analisis/Casos de Uso/CU15 - Modificando rutina de entrenamiento/TC15 - Modificando rutina de entrenamiento.xlsx
@@ -204,10 +204,6 @@
   </si>
   <si>
     <t>1. Seleccionar 'TrainerRoutiner'
-2. Seleccionar Modify Routiner'</t>
-  </si>
-  <si>
-    <t>1. Seleccionar 'TrainerRoutiner'
 2. Seleccionar Modify Routiner'
 3. Seleccionar una rutina
 4. Presionar botón Edit</t>
@@ -246,6 +242,10 @@
   <si>
     <t>Verificar:
 1. Que se actualizo la rutina en la base de datos</t>
+  </si>
+  <si>
+    <t>1. Seleccionar 'TrainerRoutiner'
+2. Seleccionar 'Modify Routiner'</t>
   </si>
 </sst>
 </file>
@@ -538,127 +538,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1202,7 +1082,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,11 +1171,11 @@
     <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -1319,7 +1199,7 @@
     <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -1329,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>15</v>
@@ -1347,17 +1227,17 @@
     <row r="5" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>15</v>
@@ -1385,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>15</v>
@@ -1403,7 +1283,7 @@
     <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -1433,11 +1313,11 @@
     <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>20</v>
@@ -1726,18 +1606,18 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="G2 G9:G23">
-    <cfRule type="cellIs" dxfId="29" priority="235" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="235" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="236" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="236" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 N9:N18">
-    <cfRule type="cellIs" dxfId="27" priority="233" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="233" stopIfTrue="1" operator="equal">
       <formula>"TEST OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="234" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="234" stopIfTrue="1" operator="equal">
       <formula>"TEST FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1850,34 +1730,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="21" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="19" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="17" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="23" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="24" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N5">
-    <cfRule type="cellIs" dxfId="15" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="21" stopIfTrue="1" operator="equal">
       <formula>"TEST OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="22" stopIfTrue="1" operator="equal">
       <formula>"TEST FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1891,10 +1771,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="13" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="18" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="19" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1917,18 +1797,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:N8">
-    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" stopIfTrue="1" operator="equal">
       <formula>"TEST OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
       <formula>"TEST FAIL"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>